<commit_message>
New test cases created
</commit_message>
<xml_diff>
--- a/MainPage.xlsx
+++ b/MainPage.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA309DF-6286-480A-AD8C-047FC11A9E40}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950AEAFF-189D-49DD-AC5D-2832670CBCDF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="MainPage" sheetId="2" r:id="rId2"/>
+    <sheet name="Main_PAGE_LOAD" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="93">
   <si>
     <t>PROJECT</t>
   </si>
@@ -141,13 +141,172 @@
   </si>
   <si>
     <t>Cookies</t>
+  </si>
+  <si>
+    <t>Scenario code</t>
+  </si>
+  <si>
+    <t>Testeed functionality</t>
+  </si>
+  <si>
+    <t>Scenario goal</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>Sulabasana</t>
+  </si>
+  <si>
+    <t>Test date</t>
+  </si>
+  <si>
+    <t>TEST_CASE_ID</t>
+  </si>
+  <si>
+    <t>TEST_CASE_NAME</t>
+  </si>
+  <si>
+    <t>TEST_CASE</t>
+  </si>
+  <si>
+    <t>PRECONDITION</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>TEST_STEPS</t>
+  </si>
+  <si>
+    <t>TEST_DATA</t>
+  </si>
+  <si>
+    <t>EXPECTED</t>
+  </si>
+  <si>
+    <t>ACTUAL</t>
+  </si>
+  <si>
+    <t>RESULT(POSITIVE/NEGATIVE)</t>
+  </si>
+  <si>
+    <t>COMMENTS</t>
+  </si>
+  <si>
+    <t>BROWSER</t>
+  </si>
+  <si>
+    <t>Ryanair main page funcionality</t>
+  </si>
+  <si>
+    <t>Verification of main page functionality</t>
+  </si>
+  <si>
+    <t>Check if all links are working, button do what is expected(i.e. fold and unfold)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attempt to load Ryanair mainpage </t>
+  </si>
+  <si>
+    <t>Internet access</t>
+  </si>
+  <si>
+    <t>Test avaialbility of Ryanair main page</t>
+  </si>
+  <si>
+    <t>1. Open web browser and provide url</t>
+  </si>
+  <si>
+    <t>url address: https://www.ryanair.com</t>
+  </si>
+  <si>
+    <t>Page loaded</t>
+  </si>
+  <si>
+    <t>MAIN_1_LOAD</t>
+  </si>
+  <si>
+    <t>MAIN_1_COOKIES</t>
+  </si>
+  <si>
+    <t>MAIN_1_RENT_A_CAR</t>
+  </si>
+  <si>
+    <t>MAIN_1_HOTELS</t>
+  </si>
+  <si>
+    <t>MAIN_1_AIRPORT_SHUTTLE</t>
+  </si>
+  <si>
+    <t>MAIN_1_PARKING</t>
+  </si>
+  <si>
+    <t>MAIN_1_CHECK_TICKET</t>
+  </si>
+  <si>
+    <t>MAIN_1_PLAN_UNFOLD</t>
+  </si>
+  <si>
+    <t>MAIN_1_BOOKING</t>
+  </si>
+  <si>
+    <t>MAIN_1_CARS</t>
+  </si>
+  <si>
+    <t>MAIN_1_SIGN_UP</t>
+  </si>
+  <si>
+    <t>MAIN_1_SIGN_IN</t>
+  </si>
+  <si>
+    <t>MAIN_1_FLIGHTS</t>
+  </si>
+  <si>
+    <t>MAIN_1_RYANAIR ROOMS</t>
+  </si>
+  <si>
+    <t>MAIN_1_CAR RENTAL</t>
+  </si>
+  <si>
+    <t>MAIN_1_HELP_CENTER</t>
+  </si>
+  <si>
+    <t>MAIN_1_ROUTE_MAP</t>
+  </si>
+  <si>
+    <t>MAIN_1_FLIGHT_SCHEDULE</t>
+  </si>
+  <si>
+    <t>MAIN_1_TRAVEL_UPDATES</t>
+  </si>
+  <si>
+    <t>MAIN_1_AIRPORTS_TRAVEL</t>
+  </si>
+  <si>
+    <t>MAIN_1_PLAN_YOUR_JOURNEY</t>
+  </si>
+  <si>
+    <t>MAIN_1_MANAGE_YOUR_JOURNEY</t>
+  </si>
+  <si>
+    <t>MAIN_1_HELPFUL_INFORMATION</t>
+  </si>
+  <si>
+    <t>MAIN_1_FOLLOW_US</t>
+  </si>
+  <si>
+    <t>MAIN_1_DOWNLOAD</t>
+  </si>
+  <si>
+    <t>Page Loaded</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +328,32 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +366,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -207,12 +402,132 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -223,12 +538,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
     <cellStyle name="Normalny 2" xfId="1" xr:uid="{6925CD86-5B7B-4A8A-8259-F25229E92425}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -506,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,12 +1248,461 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B378E2D6-9247-4F5A-B8F0-06816BD05A01}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12">
+        <v>43393</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="str">
+        <f>CONCATENATE("MAIN_1_",D37)</f>
+        <v>MAIN_1_</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D1:D6">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="zablokowany">
+      <formula>NOT(ISERROR(SEARCH("zablokowany",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="pozytywny warunkowo">
+      <formula>NOT(ISERROR(SEARCH("pozytywny warunkowo",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="pozytywny">
+      <formula>NOT(ISERROR(SEARCH("pozytywny",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="nieprzetestowano">
+      <formula>NOT(ISERROR(SEARCH("nieprzetestowano",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D6">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="negatywny">
+      <formula>NOT(ISERROR(SEARCH("negatywny",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>